<commit_message>
To: update some article viewpoint
</commit_message>
<xml_diff>
--- a/0_index.xlsx
+++ b/0_index.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haozh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_git_location\UOA_ELA_Article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8CE34A-AAC4-4B59-B0DE-AD48C3315F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E6DF08-11A7-4958-8E6F-73B1F669E2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1FC568D-D7BB-44F7-9133-FF2333D1BD27}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t>Eva Vosen</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,9 +111,6 @@
     <t>10.1007/s10676-020-09526-2</t>
   </si>
   <si>
-    <t>Is cybervetting valuable?</t>
-  </si>
-  <si>
     <t>Annika Wilcox</t>
   </si>
   <si>
@@ -273,9 +269,6 @@
   </si>
   <si>
     <t>10.1177/2053951716645828</t>
-  </si>
-  <si>
-    <t>Data-Assisted Persona Construction Using Social Media Data</t>
   </si>
   <si>
     <t>Dimitris Spiliotopoulos</t>
@@ -352,6 +345,125 @@
   </si>
   <si>
     <t>10.1177/00332941231160065</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Once an employer cyber-vets (searches for and finds information on the candidate) through a SMOS, conscious or unconscious biases such as race or gender may be applied.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.cybervetting &lt;=&gt; undermine people's trust
+2.privacy boundaries are not only important when it comes to private information, but also with information that is publicly available on social media
+3.SM data public =&gt; no context-specific &amp; data-specific expectation of privacy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>about privacy
+method: survey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>focus on young people
+method: interview
+focus on understand of SM profile checking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.young people’s understandings and deployment of social media profile checking
+2.encouraging surveillance practices as part of social media interactivity
+3.producing specific understandings of social screening.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.LinkedIn profile are not strongly correlated with organizational metrics.
+2. Taken in sum, the present findings cast serious doubts surrounding the validity of using information gleaned from within one’s LinkedIn profile in the hiring process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LinkedIn profile
+method: financial services professional,  objective sales performance metrics.
+Caution: using this information as hiring process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data-Assisted Persona Construction Using Social Media Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">talk about privacy
+method: online survey
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. young people are generally not comfortable with social media screening
+2.public information on SM cannot be fully explained by some 'traditional' variables in privacy research</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.benefits: low-cost source of information applicants
+2.talk about ethical issues, ethnic values
+3.provide an assessment of the procedural justice of social media screening and to articulate recommendations for a fairer use of social media in the selection process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>it is possible to enhance the fairness of this practice by establishing clear policies and procedures to standardize the process.
+It is therefore essential to follow some basic guidelines to address the aforementioned issues and to enhance procedural justice.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comparing applicants' attitudes across platforms showed significantly more favorable perceptions toward LinkedIn-based cybervetting than for the other three platforms.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">talk about 3 different studies
+ATC applicants' attitudes towards cybervetting
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Recruiter ratings of applicants’ Facebook information were unrelated to supervisor ratings of job performance
+2.Facebook ratings did not contribute to the prediction of these criteria beyond more traditional predictors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method: examing
+only based on facebook
+should be very cautious to use SM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.cybervetting-based ratings generally differed from applicant test scores and self-assessment ratings, employers should use caution when utilizing this pre-employment screening technique</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method: supervisors conducted cybervetting evaluations of applicant personality, cognitive ability, written communication skills, professionalism, and overall suitability
+psychometric: psychology metreics
+facebook profile only</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is cybervetting valuable?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>it is the responsibility of the organizations engaged in cybervetting to identify specific goals, develop formal policies and practices, and continuously evaluate outcomes so that negative societal consequences are minimized</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.initiate a discussion about the negative consequences of online screening and how they can be overcome
+2. stakeholders can take to manage and ameliorate harmful out_x0002_comes of cybervetting
+3. can improve the quality of individual hires. But this is untested
+4. potential to substantially undermine equal opportunity in hiring
+5. promotes privacy invasion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -422,16 +534,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,58 +859,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B5CBE1-22D2-4EA1-BE9A-571FF43022D8}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.625" customWidth="1"/>
-    <col min="2" max="2" width="94" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="8.25" customWidth="1"/>
-    <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="11.375" customWidth="1"/>
-    <col min="8" max="8" width="29.5" customWidth="1"/>
-    <col min="9" max="9" width="62" customWidth="1"/>
+    <col min="1" max="1" width="5.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23.25" style="3" customWidth="1"/>
+    <col min="9" max="9" width="43.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="40.25" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -810,20 +928,27 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -833,18 +958,25 @@
         <v>2020</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -867,9 +999,14 @@
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -892,9 +1029,14 @@
       <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -917,9 +1059,9 @@
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -942,17 +1084,22 @@
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="1">
         <v>2022</v>
@@ -965,38 +1112,43 @@
         <v>4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="1">
         <v>2022</v>
@@ -1009,19 +1161,19 @@
         <v>4</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="1">
         <v>2022</v>
@@ -1034,65 +1186,68 @@
         <v>4</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D12" s="1">
         <v>2019</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D13" s="1">
         <v>2012</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D14" s="1">
         <v>2021</v>
@@ -1105,19 +1260,24 @@
         <v>4</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1">
         <v>2020</v>
@@ -1130,19 +1290,19 @@
         <v>4</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D16" s="1">
         <v>2016</v>
@@ -1155,19 +1315,19 @@
         <v>4</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D17" s="1">
         <v>2020</v>
@@ -1180,69 +1340,79 @@
         <v>4</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D18" s="1">
         <v>2023</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D19" s="1">
         <v>2019</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D20" s="1">
         <v>2016</v>
@@ -1255,19 +1425,19 @@
         <v>4</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D21" s="1">
         <v>2022</v>
@@ -1280,19 +1450,19 @@
         <v>4</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D22" s="1">
         <v>2023</v>
@@ -1305,19 +1475,19 @@
         <v>4</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="1">
         <v>2020</v>
@@ -1330,19 +1500,19 @@
         <v>4</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D24" s="1">
         <v>2016</v>
@@ -1355,34 +1525,34 @@
         <v>4</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D25" s="1">
         <v>2022</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1390,7 +1560,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="1">
         <v>2021</v>
@@ -1403,19 +1573,19 @@
         <v>4</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>85</v>
+      <c r="B27" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27" s="1">
         <v>2023</v>
@@ -1427,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature: Evidence grid 1st version
</commit_message>
<xml_diff>
--- a/0_index.xlsx
+++ b/0_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_git_location\UOA_ELA_Article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E6DF08-11A7-4958-8E6F-73B1F669E2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9008D6-AC85-45F3-990F-3C7F5A4EDD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1FC568D-D7BB-44F7-9133-FF2333D1BD27}"/>
   </bookViews>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B5CBE1-22D2-4EA1-BE9A-571FF43022D8}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>